<commit_message>
Poll: Add view for respondent and fix bugs
</commit_message>
<xml_diff>
--- a/reports/undefined.xlsx
+++ b/reports/undefined.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>Мова программування</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+  <si>
+    <t>Яку мову программуваня ви оберете?</t>
   </si>
   <si>
     <t>Кіл-ть голосів</t>
@@ -22,22 +22,25 @@
     <t>Java</t>
   </si>
   <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
     <t>50%</t>
   </si>
   <si>
+    <t>C++</t>
+  </si>
+  <si>
     <t>JavaScript</t>
   </si>
   <si>
-    <t>C++</t>
-  </si>
-  <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Ваша оцінка</t>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>Як ви оцінюєте мову программування JavaScript?</t>
   </si>
   <si>
     <t>Середня відповідь</t>
@@ -49,10 +52,10 @@
     <t>Учасників</t>
   </si>
   <si>
-    <t>Розпочато: 21.06.2023</t>
-  </si>
-  <si>
-    <t>Закінчено: 21.06.2023</t>
+    <t>Розпочато: 22.06.2023</t>
+  </si>
+  <si>
+    <t>Закінчено: 22.06.2023</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -465,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -481,10 +484,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -495,55 +498,66 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" ht="35" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" ht="35" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>